<commit_message>
Nicholas - Updated Timesheet
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_NicholasCimino.xlsx
+++ b/Documentation/TimeSheets/TimeReport_NicholasCimino.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t xml:space="preserve">Name:</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t xml:space="preserve">Made changes to the backend to allow for communication over Wifi via HTTP requests. Successfully tested communication between Frontend and Backend Server via HTTP and Wifi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added a new JSON data model to be stored and interacted with on the database to successfully test HTTP requests from frontend to backend and display on frontend. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added port forwarding to my laptop to test slightly updated HTTP requests between frontend and backend. Helped in the development of functionality of ESP32 to send HTTP (POST) requests to the backend.</t>
   </si>
 </sst>
 </file>
@@ -628,8 +634,8 @@
   </sheetPr>
   <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -654,7 +660,7 @@
       </c>
       <c r="E1" s="4" t="n">
         <f aca="false">SUM(E4:E200)</f>
-        <v>1.31388888888889</v>
+        <v>1.70208333333333</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="6"/>
@@ -954,26 +960,46 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="A17" s="15" t="n">
+        <v>45972</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17" t="n">
+        <v>0.504861111111111</v>
+      </c>
+      <c r="D17" s="17" t="n">
+        <v>0.734722222222222</v>
+      </c>
       <c r="E17" s="13" t="n">
         <f aca="false">D17-C17</f>
-        <v>-0</v>
-      </c>
-      <c r="F17" s="14"/>
+        <v>0.229861111111111</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="A18" s="15" t="n">
+        <v>45974</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="17" t="n">
+        <v>0.517361111111111</v>
+      </c>
+      <c r="D18" s="17" t="n">
+        <v>0.675694444444445</v>
+      </c>
       <c r="E18" s="13" t="n">
         <f aca="false">D18-C18</f>
-        <v>-0</v>
-      </c>
-      <c r="F18" s="14"/>
+        <v>0.158333333333333</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>

</xml_diff>